<commit_message>
adjusted the runtime data
</commit_message>
<xml_diff>
--- a/Data/Runtime.xlsx
+++ b/Data/Runtime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\path-puzzles-solver\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D449FFA-96E9-4362-91CF-06056159540D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E07A59A-9974-43DE-A70C-2E9DA2FE3814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5235" yWindow="3945" windowWidth="18645" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t>A</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>running time (ms)</t>
+  </si>
+  <si>
+    <t>Average</t>
   </si>
 </sst>
 </file>
@@ -184,14 +187,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -474,40 +477,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4" t="s">
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="I2" s="3"/>
+      <c r="J2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3">
@@ -523,9 +546,25 @@
         <f>AVERAGE(B3:D3)</f>
         <v>1683.3333333333333</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="I3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>2.0169999999999999</v>
+      </c>
+      <c r="K3">
+        <v>2.9969999999999999</v>
+      </c>
+      <c r="L3">
+        <v>2.7450000000000001</v>
+      </c>
+      <c r="M3">
+        <f>AVERAGE(J3:L3)</f>
+        <v>2.5863333333333332</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4">
@@ -541,9 +580,25 @@
         <f t="shared" ref="E4:E28" si="0">AVERAGE(B4:D4)</f>
         <v>1321</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M28" si="1">AVERAGE(J4:L4)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B5">
@@ -559,9 +614,25 @@
         <f t="shared" si="0"/>
         <v>4199.666666666667</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="I5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>0.99</v>
+      </c>
+      <c r="K5">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="L5">
+        <v>1.9930000000000001</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6">
@@ -577,9 +648,25 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6">
+        <v>2.996</v>
+      </c>
+      <c r="K6">
+        <v>2.992</v>
+      </c>
+      <c r="L6">
+        <v>4.0030000000000001</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>3.3303333333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7">
@@ -595,9 +682,25 @@
         <f t="shared" si="0"/>
         <v>8706.6666666666661</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="I7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>0.998</v>
+      </c>
+      <c r="K7">
+        <v>0.999</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8">
@@ -613,9 +716,25 @@
         <f t="shared" si="0"/>
         <v>9161.6666666666661</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="I8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J8">
+        <v>0.97499999999999998</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B9">
@@ -631,9 +750,25 @@
         <f t="shared" si="0"/>
         <v>4056.3333333333335</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="I9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9">
+        <v>0.999</v>
+      </c>
+      <c r="K9">
+        <v>1.996</v>
+      </c>
+      <c r="L9">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>1.3320000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B10">
@@ -649,9 +784,25 @@
         <f t="shared" si="0"/>
         <v>2176.6666666666665</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="I10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J10">
+        <v>4.9859999999999998</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>5.0039999999999996</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>4.6633333333333331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B11">
@@ -667,9 +818,25 @@
         <f t="shared" si="0"/>
         <v>1354</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="I11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>4.1429999999999998</v>
+      </c>
+      <c r="K11">
+        <v>4.0110000000000001</v>
+      </c>
+      <c r="L11">
+        <v>5</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>4.3846666666666669</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B12">
@@ -685,9 +852,25 @@
         <f t="shared" si="0"/>
         <v>350.66666666666669</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="I12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>0.996</v>
+      </c>
+      <c r="K12">
+        <v>0.997</v>
+      </c>
+      <c r="L12">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>0.9956666666666667</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B13">
@@ -703,9 +886,25 @@
         <f t="shared" si="0"/>
         <v>491</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="I13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13">
+        <v>9.9960000000000004</v>
+      </c>
+      <c r="K13">
+        <v>11.000999999999999</v>
+      </c>
+      <c r="L13">
+        <v>10.007999999999999</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>10.334999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B14">
@@ -721,9 +920,25 @@
         <f t="shared" si="0"/>
         <v>9184.6666666666661</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="I14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B15">
@@ -739,9 +954,25 @@
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="I15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J15">
+        <v>27.003</v>
+      </c>
+      <c r="K15">
+        <v>27</v>
+      </c>
+      <c r="L15">
+        <v>27.998000000000001</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>27.333666666666669</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B16">
@@ -757,9 +988,25 @@
         <f t="shared" si="0"/>
         <v>318.66666666666669</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="I16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J16">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="K16">
+        <v>0.996</v>
+      </c>
+      <c r="L16">
+        <v>0.997</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>0.9993333333333333</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B17">
@@ -775,9 +1022,25 @@
         <f t="shared" si="0"/>
         <v>1671.3333333333333</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="I17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J17">
+        <v>0.995</v>
+      </c>
+      <c r="K17">
+        <v>0.995</v>
+      </c>
+      <c r="L17">
+        <v>0.99399999999999999</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>0.9946666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B18">
@@ -793,9 +1056,25 @@
         <f t="shared" si="0"/>
         <v>15.333333333333334</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="I18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B19">
@@ -811,9 +1090,25 @@
         <f t="shared" si="0"/>
         <v>2256</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="I19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0.996</v>
+      </c>
+      <c r="L19">
+        <v>0.998</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="1"/>
+        <v>0.99799999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20">
@@ -829,9 +1124,25 @@
         <f t="shared" si="0"/>
         <v>9.3333333333333339</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="I20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20">
+        <v>0.996</v>
+      </c>
+      <c r="K20">
+        <v>0.999</v>
+      </c>
+      <c r="L20">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="1"/>
+        <v>0.9986666666666667</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B21">
@@ -847,9 +1158,25 @@
         <f t="shared" si="0"/>
         <v>3051.3333333333335</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="I21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B22">
@@ -865,9 +1192,25 @@
         <f t="shared" si="0"/>
         <v>1307</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+      <c r="I22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22">
+        <v>0.94</v>
+      </c>
+      <c r="K22">
+        <v>1.0069999999999999</v>
+      </c>
+      <c r="L22">
+        <v>1.0009999999999999</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="1"/>
+        <v>0.98266666666666647</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B23">
@@ -883,9 +1226,25 @@
         <f t="shared" si="0"/>
         <v>8344.3333333333339</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="I23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <v>0</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B24">
@@ -901,9 +1260,25 @@
         <f t="shared" si="0"/>
         <v>5812</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+      <c r="I24" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B25">
@@ -919,9 +1294,25 @@
         <f t="shared" si="0"/>
         <v>8158</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="I25" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25">
+        <v>0.999</v>
+      </c>
+      <c r="K25">
+        <v>0.998</v>
+      </c>
+      <c r="L25">
+        <v>0.995</v>
+      </c>
+      <c r="M25">
+        <f t="shared" si="1"/>
+        <v>0.99733333333333329</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B26">
@@ -937,9 +1328,25 @@
         <f t="shared" si="0"/>
         <v>3388.3333333333335</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="I26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J26">
+        <v>15.000999999999999</v>
+      </c>
+      <c r="K26">
+        <v>14.994</v>
+      </c>
+      <c r="L26">
+        <v>14.992000000000001</v>
+      </c>
+      <c r="M26">
+        <f t="shared" si="1"/>
+        <v>14.995666666666665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B27">
@@ -955,9 +1362,25 @@
         <f t="shared" si="0"/>
         <v>5735.666666666667</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="I27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B28">
@@ -973,11 +1396,45 @@
         <f t="shared" si="0"/>
         <v>355</v>
       </c>
+      <c r="I28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29">
+        <f>AVERAGE(E3:E28)</f>
+        <v>3216.6923076923076</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M29">
+        <f>AVERAGE(M3:M28)</f>
+        <v>3.0224871794871793</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>